<commit_message>
increase aluop signal to 3-bits
</commit_message>
<xml_diff>
--- a/documentation/control.xlsx
+++ b/documentation/control.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="71">
   <si>
     <t>instruction</t>
   </si>
@@ -211,6 +211,27 @@
   </si>
   <si>
     <t>0/b100101</t>
+  </si>
+  <si>
+    <t>b'001101</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>2'b010</t>
+  </si>
+  <si>
+    <t>2'b000</t>
+  </si>
+  <si>
+    <t>2'bxxx</t>
+  </si>
+  <si>
+    <t>2'b011</t>
+  </si>
+  <si>
+    <t>2'b001</t>
   </si>
 </sst>
 </file>
@@ -1029,11 +1050,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1064,7 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,8 +1104,11 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
@@ -1124,8 +1148,11 @@
       <c r="M2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1154,7 +1181,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K3" s="2">
         <v>1</v>
@@ -1165,8 +1192,11 @@
       <c r="M3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1225,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>
@@ -1206,8 +1236,11 @@
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1236,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -1247,8 +1280,11 @@
       <c r="M5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1277,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -1288,8 +1324,11 @@
       <c r="M6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1318,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
@@ -1329,8 +1368,11 @@
       <c r="M7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1359,7 +1401,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -1370,13 +1412,19 @@
       <c r="M8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1405,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
@@ -1416,13 +1464,19 @@
       <c r="M10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -1462,18 +1516,27 @@
       <c r="M12" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1502,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K15" s="2">
         <v>0</v>
@@ -1513,8 +1576,11 @@
       <c r="M15" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1543,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="K16" s="2">
         <v>0</v>
@@ -1554,18 +1620,63 @@
       <c r="M16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1594,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K19" s="2">
         <v>0</v>
@@ -1605,8 +1716,11 @@
       <c r="M19" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1635,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -1646,8 +1760,11 @@
       <c r="M20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -1676,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
@@ -1687,8 +1804,11 @@
       <c r="M21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -1717,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K22" s="2">
         <v>0</v>
@@ -1728,8 +1848,11 @@
       <c r="M22" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -1758,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
@@ -1769,8 +1892,11 @@
       <c r="M23" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -1799,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
@@ -1810,8 +1936,11 @@
       <c r="M24" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1840,7 +1969,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
@@ -1851,8 +1980,11 @@
       <c r="M25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -1881,7 +2013,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="K26" s="2">
         <v>0</v>
@@ -1892,8 +2024,11 @@
       <c r="M26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -1922,7 +2057,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="K27" s="2">
         <v>0</v>
@@ -1933,13 +2068,19 @@
       <c r="M27" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
@@ -1968,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K29" s="2">
         <v>1</v>
@@ -1979,8 +2120,11 @@
       <c r="M29" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -2009,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K30" s="2">
         <v>1</v>
@@ -2018,6 +2162,9 @@
         <v>18</v>
       </c>
       <c r="M30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "support sub instruction"
This reverts commit 2421ac89e1d4dc887199baf745c20b559cb9a643.
</commit_message>
<xml_diff>
--- a/documentation/control.xlsx
+++ b/documentation/control.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>instruction</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>b'000010</t>
-  </si>
-  <si>
-    <t>0/b'100010</t>
   </si>
 </sst>
 </file>
@@ -1026,15 +1023,14 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1123,9 +1119,6 @@
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
support slti, sltui instructions
</commit_message>
<xml_diff>
--- a/documentation/control.xlsx
+++ b/documentation/control.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="80">
   <si>
     <t>instruction</t>
   </si>
@@ -216,24 +216,6 @@
     <t>b'001101</t>
   </si>
   <si>
-    <t>2'b010</t>
-  </si>
-  <si>
-    <t>2'b000</t>
-  </si>
-  <si>
-    <t>2'bxxx</t>
-  </si>
-  <si>
-    <t>2'b011</t>
-  </si>
-  <si>
-    <t>2'b001</t>
-  </si>
-  <si>
-    <t>2'b100</t>
-  </si>
-  <si>
     <t>0/b'000010</t>
   </si>
   <si>
@@ -250,6 +232,33 @@
   </si>
   <si>
     <t>0/b'101001</t>
+  </si>
+  <si>
+    <t>b'001010</t>
+  </si>
+  <si>
+    <t>3'b101</t>
+  </si>
+  <si>
+    <t>b'001001</t>
+  </si>
+  <si>
+    <t>3'b010</t>
+  </si>
+  <si>
+    <t>3'bxxx</t>
+  </si>
+  <si>
+    <t>3'b001</t>
+  </si>
+  <si>
+    <t>3'b000</t>
+  </si>
+  <si>
+    <t>3'b011</t>
+  </si>
+  <si>
+    <t>3'b100</t>
   </si>
 </sst>
 </file>
@@ -1076,9 +1085,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9:O9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1132,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -1167,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
@@ -1214,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
@@ -1261,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
@@ -1308,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
@@ -1355,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
@@ -1402,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L7" s="2">
         <v>0</v>
@@ -1449,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L8" s="2">
         <v>0</v>
@@ -1469,7 +1478,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1496,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L9" s="2">
         <v>0</v>
@@ -1543,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L10" s="2">
         <v>0</v>
@@ -1563,7 +1572,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1590,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="L11" s="2">
         <v>0</v>
@@ -1637,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L12" s="2">
         <v>0</v>
@@ -1656,11 +1665,44 @@
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
       <c r="I13" s="2">
         <v>0</v>
       </c>
       <c r="J13" s="2">
         <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O13" s="2">
         <v>1</v>
@@ -1670,11 +1712,44 @@
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
       <c r="I14" s="2">
         <v>0</v>
       </c>
       <c r="J14" s="2">
         <v>0</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="O14" s="2">
         <v>0</v>
@@ -1712,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
@@ -1759,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1806,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -1826,7 +1901,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>16</v>
@@ -1852,8 +1927,8 @@
       <c r="J18" s="4">
         <v>0</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>18</v>
+      <c r="K18" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="L18" s="4">
         <v>0</v>
@@ -1900,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
@@ -1947,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -1994,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L21" s="2">
         <v>0</v>
@@ -2041,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L22" s="2">
         <v>0</v>
@@ -2088,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -2135,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L24" s="2">
         <v>0</v>
@@ -2182,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
@@ -2229,7 +2304,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L26" s="2">
         <v>0</v>
@@ -2276,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L27" s="2">
         <v>0</v>
@@ -2296,7 +2371,7 @@
         <v>57</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>18</v>
@@ -2323,7 +2398,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
@@ -2370,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L29" s="2">
         <v>1</v>
@@ -2417,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L30" s="2">
         <v>1</v>

</xml_diff>